<commit_message>
aghensi@20160704 bugfix import e processing (excel, tuple e database) - dati in uscita inverosimili!
</commit_message>
<xml_diff>
--- a/resources/deercreek.xlsx
+++ b/resources/deercreek.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geo!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">geo!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -216,7 +216,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -501,16 +500,16 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
@@ -696,14 +695,14 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>167.94</v>
       </c>
       <c r="C4" s="5">
-        <v>800</v>
+        <v>4597.3999999999996</v>
       </c>
       <c r="D4">
         <f>C4-B4</f>
-        <v>800</v>
+        <v>4429.46</v>
       </c>
       <c r="E4">
         <v>0.86</v>
@@ -729,10 +728,10 @@
       <c r="L4">
         <v>0.5</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>6206</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>12589</v>
       </c>
       <c r="O4">
@@ -775,14 +774,16 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <f>B4</f>
+        <v>167.94</v>
       </c>
       <c r="C5" s="5">
-        <v>800</v>
+        <f>C4</f>
+        <v>4597.3999999999996</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D8" si="0">C5-B5</f>
-        <v>800</v>
+        <v>4429.46</v>
       </c>
       <c r="E5">
         <v>0.14000000000000001</v>
@@ -808,10 +809,10 @@
       <c r="L5">
         <v>0.5</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>6202</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>22410</v>
       </c>
       <c r="O5">
@@ -854,14 +855,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="8">
-        <v>800</v>
+        <f>C5</f>
+        <v>4597.3999999999996</v>
       </c>
       <c r="C6" s="8">
-        <v>850</v>
+        <f>B6+18.7</f>
+        <v>4616.0999999999995</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>18.699999999999818</v>
       </c>
       <c r="E6" s="8">
         <v>1</v>
@@ -872,17 +875,33 @@
       <c r="G6" s="8">
         <v>20</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="6">
+        <v>23.56</v>
+      </c>
       <c r="I6" s="8">
         <v>13.8</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="9">
+        <v>6202</v>
+      </c>
+      <c r="N6" s="9">
+        <v>6206</v>
+      </c>
+      <c r="O6">
+        <v>1.5</v>
+      </c>
+      <c r="P6">
+        <v>1.7</v>
+      </c>
       <c r="Q6">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -899,8 +918,12 @@
       <c r="U6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="V6">
+        <v>3.45</v>
+      </c>
+      <c r="W6">
+        <v>4.83</v>
+      </c>
       <c r="X6">
         <v>0.7</v>
       </c>
@@ -937,14 +960,15 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>850</v>
+        <f>C6</f>
+        <v>4616.0999999999995</v>
       </c>
       <c r="C7">
-        <v>1000</v>
+        <v>6498</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>1881.9000000000005</v>
       </c>
       <c r="E7">
         <v>0.86</v>
@@ -970,10 +994,10 @@
       <c r="L7">
         <v>0.5</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>6206</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>12589</v>
       </c>
       <c r="O7">
@@ -1016,14 +1040,16 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>850</v>
+        <f>B7</f>
+        <v>4616.0999999999995</v>
       </c>
       <c r="C8">
-        <v>1000</v>
+        <f>C7</f>
+        <v>6498</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>1881.9000000000005</v>
       </c>
       <c r="E8">
         <v>0.14000000000000001</v>
@@ -1049,10 +1075,10 @@
       <c r="L8">
         <v>0.5</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>6202</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <v>22410</v>
       </c>
       <c r="O8">

</xml_diff>

<commit_message>
fixed multiple material selection in main_loop_pool.py geology parameters modified
</commit_message>
<xml_diff>
--- a/resources/deercreek.xlsx
+++ b/resources/deercreek.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geo!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">geo!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>fine</t>
   </si>
@@ -124,13 +124,16 @@
   </si>
   <si>
     <t>ei_max</t>
+  </si>
+  <si>
+    <t>Gpa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +146,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -206,12 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -498,10 +491,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:AX14"/>
+  <dimension ref="A1:AX8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,8 +595,12 @@
       </c>
       <c r="K2"/>
       <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2" s="2"/>
@@ -614,79 +611,79 @@
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="X3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Y3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -697,7 +694,7 @@
       <c r="B4">
         <v>167.94</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>4597.3999999999996</v>
       </c>
       <c r="D4">
@@ -710,10 +707,10 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>19.95</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>26.55</v>
       </c>
       <c r="I4">
@@ -728,11 +725,11 @@
       <c r="L4">
         <v>0.5</v>
       </c>
-      <c r="M4" s="9">
-        <v>6206</v>
-      </c>
-      <c r="N4" s="9">
-        <v>12589</v>
+      <c r="M4" s="7">
+        <v>6.2060000000000004</v>
+      </c>
+      <c r="N4" s="7">
+        <v>12.589</v>
       </c>
       <c r="O4">
         <v>1.5</v>
@@ -742,16 +739,16 @@
       </c>
       <c r="Q4">
         <f>S4-5</f>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U4" t="s">
         <v>18</v>
@@ -777,7 +774,7 @@
         <f>B4</f>
         <v>167.94</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <f>C4</f>
         <v>4597.3999999999996</v>
       </c>
@@ -791,10 +788,10 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>23.56</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>25.13</v>
       </c>
       <c r="I5">
@@ -809,11 +806,11 @@
       <c r="L5">
         <v>0.5</v>
       </c>
-      <c r="M5" s="9">
-        <v>6202</v>
-      </c>
-      <c r="N5" s="9">
-        <v>22410</v>
+      <c r="M5" s="7">
+        <v>6.202</v>
+      </c>
+      <c r="N5" s="7">
+        <v>22.41</v>
       </c>
       <c r="O5">
         <v>1.7</v>
@@ -823,16 +820,16 @@
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q8" si="1">S5-5</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S5">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U5" t="s">
         <v>19</v>
@@ -851,50 +848,50 @@
       </c>
     </row>
     <row r="6" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <f>C5</f>
         <v>4597.3999999999996</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <f>B6+18.7</f>
         <v>4616.0999999999995</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>18.699999999999818</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>20</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>23.56</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>13.8</v>
       </c>
       <c r="J6">
         <v>30</v>
       </c>
       <c r="K6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>0.5</v>
       </c>
-      <c r="M6" s="9">
-        <v>6202</v>
-      </c>
-      <c r="N6" s="9">
-        <v>6206</v>
+      <c r="M6" s="7">
+        <v>2</v>
+      </c>
+      <c r="N6" s="7">
+        <v>3</v>
       </c>
       <c r="O6">
         <v>1.5</v>
@@ -906,16 +903,16 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="R6" s="8">
-        <v>0</v>
-      </c>
-      <c r="S6" s="8">
+      <c r="R6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="S6" s="6">
         <v>45</v>
       </c>
-      <c r="T6" s="8">
-        <v>0</v>
-      </c>
-      <c r="U6" s="8" t="s">
+      <c r="T6" s="6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="V6">
@@ -976,10 +973,10 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>19.95</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>26.55</v>
       </c>
       <c r="I7">
@@ -994,11 +991,11 @@
       <c r="L7">
         <v>0.5</v>
       </c>
-      <c r="M7" s="9">
-        <v>6206</v>
-      </c>
-      <c r="N7" s="9">
-        <v>12589</v>
+      <c r="M7" s="7">
+        <v>6.2060000000000004</v>
+      </c>
+      <c r="N7" s="7">
+        <v>12.589</v>
       </c>
       <c r="O7">
         <v>1.5</v>
@@ -1008,16 +1005,16 @@
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S7">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U7" t="s">
         <v>18</v>
@@ -1057,10 +1054,10 @@
       <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>23.56</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>25.13</v>
       </c>
       <c r="I8">
@@ -1075,11 +1072,11 @@
       <c r="L8">
         <v>0.5</v>
       </c>
-      <c r="M8" s="9">
-        <v>6202</v>
-      </c>
-      <c r="N8" s="9">
-        <v>22410</v>
+      <c r="M8" s="7">
+        <v>6.202</v>
+      </c>
+      <c r="N8" s="7">
+        <v>22.41</v>
       </c>
       <c r="O8">
         <v>1.7</v>
@@ -1089,16 +1086,16 @@
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S8">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U8" t="s">
         <v>19</v>
@@ -1115,17 +1112,6 @@
       <c r="Y8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="G10">
-        <v>0.157087</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="AV11" s="4"/>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="S14" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A4:BA15">

</xml_diff>